<commit_message>
Diamond jewellery Bullion jewellery --- NosePin -- 		listing gold weight 		with and without diamond arrangement 		gold weight field removed 		combination -- Gold and polki added 		result page polki added 		diamond proce/carat , value of diamond, gemstone price / carat, value of gemstone , labour charge, other material 		on gold click gold type shown 		net weight + gross weight 		on polki select combination chooses gold and polki city added on gaining details of vendor
</commit_message>
<xml_diff>
--- a/sampleJewelleryList.xlsx
+++ b/sampleJewelleryList.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\iftosi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\iftosi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Product details</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Diamonds</t>
   </si>
   <si>
-    <t>Shape</t>
-  </si>
-  <si>
     <t>Clarity</t>
   </si>
   <si>
@@ -96,19 +93,43 @@
     <t>Price</t>
   </si>
   <si>
-    <t>dsdsd</t>
-  </si>
-  <si>
-    <t>bfdg</t>
-  </si>
-  <si>
-    <t>vdvcxvx</t>
+    <t>G</t>
+  </si>
+  <si>
+    <t>IGI</t>
+  </si>
+  <si>
+    <t>BlueStone</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Rings</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>White Gold</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>Emerald</t>
+  </si>
+  <si>
+    <t>Ring for Upload</t>
+  </si>
+  <si>
+    <t>AGS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -722,6 +743,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -757,6 +795,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -911,11 +966,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" customWidth="1"/>
+    <col min="18" max="18" width="17.140625" customWidth="1"/>
+    <col min="19" max="19" width="17.5703125" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" customWidth="1"/>
+    <col min="23" max="23" width="13" customWidth="1"/>
+    <col min="24" max="24" width="17.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -958,66 +1029,114 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B2">
-        <v>2324</v>
+        <v>1002324</v>
       </c>
       <c r="C2">
         <v>1000</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F2">
-        <v>45645</v>
+        <v>14</v>
       </c>
       <c r="G2">
         <v>56</v>
       </c>
       <c r="H2">
         <v>100</v>
+      </c>
+      <c r="I2">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2">
+        <v>12</v>
+      </c>
+      <c r="L2">
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2">
+        <v>12.12</v>
+      </c>
+      <c r="P2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2">
+        <v>12</v>
+      </c>
+      <c r="R2">
+        <v>2</v>
+      </c>
+      <c r="S2">
+        <v>12</v>
+      </c>
+      <c r="T2">
+        <v>2121</v>
+      </c>
+      <c r="U2">
+        <v>123</v>
+      </c>
+      <c r="V2" t="s">
+        <v>34</v>
+      </c>
+      <c r="W2" t="s">
+        <v>25</v>
+      </c>
+      <c r="X2" t="s">
+        <v>26</v>
       </c>
       <c r="Y2">
         <v>152000</v>

</xml_diff>

<commit_message>
three excel product files with filters implemented
</commit_message>
<xml_diff>
--- a/sampleJewelleryList.xlsx
+++ b/sampleJewelleryList.xlsx
@@ -9,14 +9,13 @@
   </bookViews>
   <sheets>
     <sheet name="Jewellery" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
   <si>
     <t>Category</t>
   </si>
@@ -132,43 +131,7 @@
     <t>GOLD,DIAMONDS &amp; GEMSTONES</t>
   </si>
   <si>
-    <t>GOLD &amp; DIAMONDS</t>
-  </si>
-  <si>
-    <t>PLATINUM &amp; DIAMONDS</t>
-  </si>
-  <si>
-    <t>SILVER &amp; DIAMONDS</t>
-  </si>
-  <si>
-    <t>SILVER,DIAMONDS &amp; GEMSTONES</t>
-  </si>
-  <si>
-    <t>GOLD &amp; GEMSTONES</t>
-  </si>
-  <si>
-    <t>SILVER &amp; GEMSTONES</t>
-  </si>
-  <si>
-    <t>GOLD &amp; SWAROVSKI ZIRCONIA</t>
-  </si>
-  <si>
-    <t>SILVER &amp; SWAROVSKI ZIRCONIA</t>
-  </si>
-  <si>
-    <t>GOLD &amp; CZ</t>
-  </si>
-  <si>
-    <t>SILVER &amp; CZ</t>
-  </si>
-  <si>
-    <t>PLAIN GOLD</t>
-  </si>
-  <si>
-    <t>PLAIN PLATINUM</t>
-  </si>
-  <si>
-    <t>PLAIN SILVER</t>
+    <t> </t>
   </si>
 </sst>
 </file>
@@ -270,13 +233,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG10"/>
+  <dimension ref="A1:AG65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.8542510121458"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.1417004048583"/>
@@ -427,66 +390,222 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="1" t="s">
-        <v>34</v>
+    <row r="1048576" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF1048576" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG1048576" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="8">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F1:F10" type="list">
+  <dataValidations count="23">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F1" type="list">
       <formula1>"Gold,Silver,Platinum"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G1:G10" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G1" type="list">
       <formula1>"White,Yellow,Pink"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H1:H10 O1:O10" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H1 O1" type="list">
       <formula1>"D,E,F,G,H,I,J,K,L,M,N,O"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I1:I10 N1:N10" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I1 N1" type="list">
       <formula1>"IF,VVS1,VVS2,VS1,VS2,SI1,SI2,I1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J1:J10 P1:P10 U1:U10 Y1:Y10 AE1:AF10" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J1 P1 U1 Y1 AE1:AF1" type="decimal">
       <formula1>0</formula1>
       <formula2>99999.99</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K1:L10 R1:S10 V1:W10 Z1:Z10 AG1:AG10" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K1:L1 R1:S1 V1:W1 Z1 AG1" type="decimal">
       <formula1>0</formula1>
       <formula2>9999999.99</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M1:M10" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M1" type="list">
       <formula1>"Round,Pear,Emerald,Asscher,Princess,Marquise,Oval,Cushion,Heart,Radiant"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T1:T10" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T1" type="list">
       <formula1>"AMBER,AMETHYST,AQUAMARINE,BLUE TOPAZ,CORAL,EMERALD,GARNET,GOLDEN TOPAZ,HYDRO,IOLITE,LEMON TOPAZ,MOONSTONE,ONYX,OPAL,PEARL,PERIDOT,ROSE QUARTZ,RUBILITE,RUBY,SAPPHIRE,SMOKY TOPAZ,TANZANITE,TURQUOISE"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1048576" type="list">
+      <formula1>"Rings,Earrings,Pendants,Necklaces,Bangles/Bracelets,NosePin,Polki/Jadau,Mangalsutra"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C1048576" type="list">
+      <formula1>"GOLD &amp; DIAMONDS,PLATINUM &amp; DIAMONDS,SILVER &amp; DIAMONDS,GOLD,DIAMONDS &amp; GEMSTONES,PLATINUM,DIAMONDS &amp; GEMSTONES,SILVER,DIAMONDS &amp; GEMSTONES,GOLD &amp; GEMSTONES,SILVER &amp; GEMSTONES,GOLD &amp; SWAROVSKI ZIRCONIA,SILVER &amp; SWAROVSKI ZIRCONIA,GOLD &amp; CZ,SILVER &amp; CZ,PLAIN GOLD,PLAIN PLATINUM,PLAIN SILVER,GOLD &amp; POLKI"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D1048576" type="list">
+      <formula1>"SGL,DGLA,EGL,IGI,BIS,NONE,Other"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F2:F1048576" type="list">
+      <formula1>"Gold,Silver,Platinum"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G2:G1048576" type="list">
+      <formula1>"White,Yellow,Pink"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H2:H1048576" type="list">
+      <formula1>"D,E,F,G,H,I,J,K,L,M,N,O"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I2:I1048576" type="list">
+      <formula1>"IF,VVS1,VVS2,VS1,VS2,SI1,SI2,I1"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J2:J1048576 P2:P1048576 U2:U1048576 Y2:Y1048576 AE2:AF1048576" type="decimal">
+      <formula1>0</formula1>
+      <formula2>99999.99</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K2:L1048576 R2:S1048576 V2:W1048576 Z2:Z1048576 AG2:AG1048576" type="decimal">
+      <formula1>0</formula1>
+      <formula2>9999999.99</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M2:M1048576" type="list">
+      <formula1>"Round,Pear,Emerald,Asscher,Princess,Marquise,Oval,Cushion,Heart,Radiant"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N2:N1048576" type="list">
+      <formula1>"IF,VVS1,VVS2,VS1,VS2,SI1,SI2,I1"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O2:O1048576" type="list">
+      <formula1>"D,E,F,G,H,I,J,K,L,M,N,O"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q2:Q1048576 X2:X1048576" type="whole">
+      <formula1>0</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T2:T1048576" type="list">
+      <formula1>"AMBER,AMETHYST,AQUAMARINE,BLUE TOPAZ,CORAL,EMERALD,GARNET,GOLDEN TOPAZ,HYDRO,IOLITE,LEMON TOPAZ,MOONSTONE,ONYX,OPAL,PEARL,PERIDOT,ROSE QUARTZ,RUBILITE,RUBY,SAPPHIRE,SMOKY TOPAZ,TANZANITE,TURQUOISE"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AC2:AC1048576" type="list">
+      <formula1>"12,14,18,20,22,24,995,999,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -498,110 +617,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="YP34:YP48"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.2834008097166"/>
-    <col collapsed="false" hidden="false" max="665" min="5" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="666" min="666" style="0" width="36.5708502024291"/>
-    <col collapsed="false" hidden="false" max="1025" min="667" style="0" width="8.5748987854251"/>
-  </cols>
-  <sheetData>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="YP34" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="YP35" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="YP36" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="YP37" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="YP38" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="YP39" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="YP40" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="YP41" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="YP42" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="YP43" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="YP44" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="YP45" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="YP46" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="YP47" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="YP48" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>